<commit_message>
Corrida | SFE-ASF | 2026-01-20 12:54:11.344913
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Usuario</t>
   </si>
   <si>
-    <t xml:space="preserve">focampo</t>
+    <t xml:space="preserve">pcohan</t>
   </si>
   <si>
     <t xml:space="preserve">fecha</t>
@@ -14908,4 +14908,237 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7cec21613a3259523bdab11a1e26aca">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68943c349d3a016936c8f8cb3335004b" ns2:_="" ns3:_="">
+    <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
+    <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5dd4176-d247-4204-85b8-921214f3ccea" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="01529062-7a8b-4d76-943d-e0db5644ee6d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359b39ce-e1f9-4933-8424-33b611e6fdcd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9b73259-0823-4f05-8927-4a40ee49fbe1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="359b39ce-e1f9-4933-8424-33b611e6fdcd">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FEFD466-5733-4DF3-834F-F7CD114FCCA5}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDDBD16A-3CBC-40AC-846E-DBF926AE5C64}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA6E42A3-7503-4E0A-82AE-C2CE7D5EEDB5}"/>
 </file>
</xml_diff>

<commit_message>
Corrida | SFE-ASF | 2026-01-23 08:45:00.466092
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Fecha</t>
   </si>
   <si>
-    <t xml:space="preserve">20/01/2026</t>
+    <t xml:space="preserve">23/01/2026</t>
   </si>
   <si>
     <t xml:space="preserve">Usuario</t>
@@ -1525,7 +1525,7 @@
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9" t="n">
-        <v>0.492683742945254</v>
+        <v>0.493373722540264</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -1583,7 +1583,7 @@
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" t="n">
-        <v>0.18842599319823</v>
+        <v>0.189836777363751</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -1653,7 +1653,7 @@
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18" t="n">
-        <v>0.12725141395767</v>
+        <v>0.107692456131355</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
@@ -1683,7 +1683,7 @@
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20" t="n">
-        <v>0.0198186057878541</v>
+        <v>0.0204454898579549</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -14736,7 +14736,7 @@
         <v>306</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>-0.136995911235706</v>
+        <v>-0.13844653763458</v>
       </c>
     </row>
     <row r="6">
@@ -14744,7 +14744,7 @@
         <v>307</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>-0.0451936931603418</v>
+        <v>-0.0459268839515573</v>
       </c>
     </row>
     <row r="7">
@@ -14752,7 +14752,7 @@
         <v>308</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.0541225511249317</v>
+        <v>0.0530652384810557</v>
       </c>
     </row>
     <row r="8">
@@ -14760,7 +14760,7 @@
         <v>309</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.144027912883594</v>
+        <v>0.141777005563421</v>
       </c>
     </row>
     <row r="9">
@@ -14768,7 +14768,7 @@
         <v>310</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.259522005288736</v>
+        <v>0.259377658506186</v>
       </c>
     </row>
     <row r="10">
@@ -14776,7 +14776,7 @@
         <v>311</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.375747393077601</v>
+        <v>0.37893641892541</v>
       </c>
     </row>
     <row r="11">
@@ -14784,7 +14784,7 @@
         <v>312</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.447139939309563</v>
+        <v>0.449065592741075</v>
       </c>
     </row>
     <row r="12">
@@ -14792,7 +14792,7 @@
         <v>313</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>0.488267866754336</v>
+        <v>0.487711803405923</v>
       </c>
     </row>
     <row r="13">
@@ -14800,7 +14800,7 @@
         <v>314</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.492683742945254</v>
+        <v>0.493373722540264</v>
       </c>
     </row>
     <row r="14">
@@ -14808,7 +14808,7 @@
         <v>315</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.434080629835322</v>
+        <v>0.435702624921804</v>
       </c>
     </row>
     <row r="15">
@@ -14816,7 +14816,7 @@
         <v>316</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.306043245356789</v>
+        <v>0.306159409083136</v>
       </c>
     </row>
     <row r="16">
@@ -14824,7 +14824,7 @@
         <v>317</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.168326254037459</v>
+        <v>0.168769145660554</v>
       </c>
     </row>
     <row r="17">
@@ -14832,7 +14832,7 @@
         <v>318</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.0498973203610863</v>
+        <v>0.0512540591362047</v>
       </c>
     </row>
     <row r="18">
@@ -14840,7 +14840,7 @@
         <v>319</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>-0.019344470399186</v>
+        <v>-0.0198621218742659</v>
       </c>
     </row>
     <row r="19">
@@ -14848,7 +14848,7 @@
         <v>320</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>-0.0201248798294758</v>
+        <v>-0.0210010112024413</v>
       </c>
     </row>
     <row r="20">
@@ -14856,7 +14856,7 @@
         <v>321</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>-0.0425036742249541</v>
+        <v>-0.0409367940429145</v>
       </c>
     </row>
     <row r="21">
@@ -14864,7 +14864,7 @@
         <v>322</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>-0.109711486812074</v>
+        <v>-0.10870776385011</v>
       </c>
     </row>
     <row r="22">
@@ -14872,7 +14872,7 @@
         <v>323</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>-0.130287410505407</v>
+        <v>-0.132356335534</v>
       </c>
     </row>
     <row r="23">
@@ -14880,7 +14880,7 @@
         <v>324</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>-0.0680506904213139</v>
+        <v>-0.0701536831329255</v>
       </c>
     </row>
     <row r="24">
@@ -15123,22 +15123,22 @@
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1F02F79-030C-466E-AA28-028B5BBD901D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90484F79-802C-4AEF-B3DF-331608F4536A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{411767A1-91B3-47D0-9926-F5ADCFB26489}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0141A135-D7AB-42A3-9871-8E790C90D9E4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFB2AF50-A694-42D6-ACBE-B36539C865FB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F8C992-826F-477E-8BD4-1A7D2B99D09A}"/>
 </file>
</xml_diff>

<commit_message>
Corrida | SFE-ESC1 | 2026-02-02 10:06:50.662589
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -14944,4 +14944,237 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7cec21613a3259523bdab11a1e26aca">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68943c349d3a016936c8f8cb3335004b" ns2:_="" ns3:_="">
+    <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
+    <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5dd4176-d247-4204-85b8-921214f3ccea" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="01529062-7a8b-4d76-943d-e0db5644ee6d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359b39ce-e1f9-4933-8424-33b611e6fdcd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9b73259-0823-4f05-8927-4a40ee49fbe1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="359b39ce-e1f9-4933-8424-33b611e6fdcd">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DF4B21E-14C2-4A3C-86DA-407EB5032A91}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F83ABC8-A014-4E76-8EF2-375CAF16C5BE}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BF3EC8D-2642-4E5C-A03F-9D38BF23CC80}"/>
 </file>
</xml_diff>

<commit_message>
Corrida | SFE-ID | 2026-02-09 10:24:56.076534
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -14944,4 +14944,237 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7cec21613a3259523bdab11a1e26aca">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68943c349d3a016936c8f8cb3335004b" ns2:_="" ns3:_="">
+    <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
+    <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5dd4176-d247-4204-85b8-921214f3ccea" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="01529062-7a8b-4d76-943d-e0db5644ee6d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359b39ce-e1f9-4933-8424-33b611e6fdcd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9b73259-0823-4f05-8927-4a40ee49fbe1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="359b39ce-e1f9-4933-8424-33b611e6fdcd">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E02702EA-D55F-4928-A5C7-AB50D7BD73B0}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C736AD06-A8E8-48C9-AF83-5392FFB81587}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98A28AAA-1EB3-4771-A122-2FB259342DF0}"/>
 </file>
</xml_diff>

<commit_message>
Corrida | SFE-ASF | 2026-02-09 10:38:36.360199
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Usuario</t>
   </si>
   <si>
-    <t xml:space="preserve">focampo</t>
+    <t xml:space="preserve">pcohan</t>
   </si>
   <si>
     <t xml:space="preserve">fecha</t>
@@ -14944,237 +14944,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7cec21613a3259523bdab11a1e26aca">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68943c349d3a016936c8f8cb3335004b" ns2:_="" ns3:_="">
-    <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
-    <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5dd4176-d247-4204-85b8-921214f3ccea" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="01529062-7a8b-4d76-943d-e0db5644ee6d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359b39ce-e1f9-4933-8424-33b611e6fdcd" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9b73259-0823-4f05-8927-4a40ee49fbe1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="359b39ce-e1f9-4933-8424-33b611e6fdcd">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E02702EA-D55F-4928-A5C7-AB50D7BD73B0}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C736AD06-A8E8-48C9-AF83-5392FFB81587}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98A28AAA-1EB3-4771-A122-2FB259342DF0}"/>
 </file>
</xml_diff>

<commit_message>
Corrida | SFE-ID | 2026-02-09 10:39:36.36413
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -14944,4 +14944,237 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7cec21613a3259523bdab11a1e26aca">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68943c349d3a016936c8f8cb3335004b" ns2:_="" ns3:_="">
+    <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
+    <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5dd4176-d247-4204-85b8-921214f3ccea" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="01529062-7a8b-4d76-943d-e0db5644ee6d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359b39ce-e1f9-4933-8424-33b611e6fdcd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9b73259-0823-4f05-8927-4a40ee49fbe1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="359b39ce-e1f9-4933-8424-33b611e6fdcd">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95BFF6C7-78B1-4509-965A-500CB73ECDB6}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6FD168D-2F5C-476A-B027-D1DEB5E2E661}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59FBC877-808C-48C1-839F-C4B0BF500A4A}"/>
 </file>
</xml_diff>

<commit_message>
Corrida | SFE-ASF | 2026-02-12 15:34:09.348041
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Fecha</t>
   </si>
   <si>
-    <t xml:space="preserve">09/02/2026</t>
+    <t xml:space="preserve">12/02/2026</t>
   </si>
   <si>
     <t xml:space="preserve">Usuario</t>
@@ -14944,237 +14944,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7cec21613a3259523bdab11a1e26aca">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68943c349d3a016936c8f8cb3335004b" ns2:_="" ns3:_="">
-    <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
-    <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5dd4176-d247-4204-85b8-921214f3ccea" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="01529062-7a8b-4d76-943d-e0db5644ee6d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359b39ce-e1f9-4933-8424-33b611e6fdcd" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9b73259-0823-4f05-8927-4a40ee49fbe1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="359b39ce-e1f9-4933-8424-33b611e6fdcd">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95BFF6C7-78B1-4509-965A-500CB73ECDB6}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6FD168D-2F5C-476A-B027-D1DEB5E2E661}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59FBC877-808C-48C1-839F-C4B0BF500A4A}"/>
 </file>
</xml_diff>

<commit_message>
Corrida | SFE-ASF | 2026-02-13 08:45:18.800646
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -106,13 +106,13 @@
     <t xml:space="preserve">Fecha</t>
   </si>
   <si>
-    <t xml:space="preserve">12/02/2026</t>
+    <t xml:space="preserve">13/02/2026</t>
   </si>
   <si>
     <t xml:space="preserve">Usuario</t>
   </si>
   <si>
-    <t xml:space="preserve">pcohan</t>
+    <t xml:space="preserve">focampo</t>
   </si>
   <si>
     <t xml:space="preserve">fecha</t>
@@ -1525,7 +1525,7 @@
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9" t="n">
-        <v>0.538718537523096</v>
+        <v>0.537290771448983</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -1583,7 +1583,7 @@
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" t="n">
-        <v>0.242285451624975</v>
+        <v>0.239400992938853</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -1653,7 +1653,7 @@
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18" t="n">
-        <v>0.128867689672822</v>
+        <v>0.12358163512308</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
@@ -1683,7 +1683,7 @@
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20" t="n">
-        <v>0.329730862756446</v>
+        <v>0.327332397469789</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -14772,7 +14772,7 @@
         <v>306</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>-0.153196931258976</v>
+        <v>-0.152582126386725</v>
       </c>
     </row>
     <row r="6">
@@ -14780,7 +14780,7 @@
         <v>307</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>-0.0715745155561449</v>
+        <v>-0.0706603053203405</v>
       </c>
     </row>
     <row r="7">
@@ -14788,7 +14788,7 @@
         <v>308</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.0305801656025711</v>
+        <v>0.0308903820241811</v>
       </c>
     </row>
     <row r="8">
@@ -14796,7 +14796,7 @@
         <v>309</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.126801457531059</v>
+        <v>0.125613878078508</v>
       </c>
     </row>
     <row r="9">
@@ -14804,7 +14804,7 @@
         <v>310</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.258264399789519</v>
+        <v>0.256977499298484</v>
       </c>
     </row>
     <row r="10">
@@ -14812,7 +14812,7 @@
         <v>311</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.409944540233078</v>
+        <v>0.409475224591772</v>
       </c>
     </row>
     <row r="11">
@@ -14820,7 +14820,7 @@
         <v>312</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.48584007626918</v>
+        <v>0.486018887479727</v>
       </c>
     </row>
     <row r="12">
@@ -14828,7 +14828,7 @@
         <v>313</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>0.51184353059561</v>
+        <v>0.512108674213389</v>
       </c>
     </row>
     <row r="13">
@@ -14836,7 +14836,7 @@
         <v>314</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.538718537523096</v>
+        <v>0.537290771448983</v>
       </c>
     </row>
     <row r="14">
@@ -14844,7 +14844,7 @@
         <v>315</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.492225001015771</v>
+        <v>0.489286207591072</v>
       </c>
     </row>
     <row r="15">
@@ -14852,7 +14852,7 @@
         <v>316</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.344423664912825</v>
+        <v>0.343425432530259</v>
       </c>
     </row>
     <row r="16">
@@ -14860,7 +14860,7 @@
         <v>317</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.188453671687091</v>
+        <v>0.187699024710436</v>
       </c>
     </row>
     <row r="17">
@@ -14868,7 +14868,7 @@
         <v>318</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.0509527036925829</v>
+        <v>0.0504220257927692</v>
       </c>
     </row>
     <row r="18">
@@ -14876,7 +14876,7 @@
         <v>319</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>-0.0230421520667761</v>
+        <v>-0.0238287101109297</v>
       </c>
     </row>
     <row r="19">
@@ -14884,7 +14884,7 @@
         <v>320</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>-0.027451076280233</v>
+        <v>-0.0268494823746423</v>
       </c>
     </row>
     <row r="20">
@@ -14892,7 +14892,7 @@
         <v>321</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>-0.0730442224554981</v>
+        <v>-0.0689686484154335</v>
       </c>
     </row>
     <row r="21">
@@ -14900,7 +14900,7 @@
         <v>322</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>-0.124977171866364</v>
+        <v>-0.122665475641747</v>
       </c>
     </row>
     <row r="22">
@@ -14908,7 +14908,7 @@
         <v>323</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>-0.119861441761191</v>
+        <v>-0.11600813826808</v>
       </c>
     </row>
     <row r="23">
@@ -14916,7 +14916,7 @@
         <v>324</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>-0.0926906754421506</v>
+        <v>-0.0881890063500632</v>
       </c>
     </row>
     <row r="24">

</xml_diff>

<commit_message>
Corrida | GLO-BARC | 2026-02-13 09:21:43.757393
</commit_message>
<xml_diff>
--- a/web_ces/indicadores/SFE-ASF_out.xlsx
+++ b/web_ces/indicadores/SFE-ASF_out.xlsx
@@ -14944,4 +14944,237 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7cec21613a3259523bdab11a1e26aca">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68943c349d3a016936c8f8cb3335004b" ns2:_="" ns3:_="">
+    <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
+    <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b5dd4176-d247-4204-85b8-921214f3ccea" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="01529062-7a8b-4d76-943d-e0db5644ee6d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359b39ce-e1f9-4933-8424-33b611e6fdcd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c9b73259-0823-4f05-8927-4a40ee49fbe1}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="359b39ce-e1f9-4933-8424-33b611e6fdcd">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5dd4176-d247-4204-85b8-921214f3ccea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="359b39ce-e1f9-4933-8424-33b611e6fdcd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA2ACB8-709A-4EC3-8889-63891AE4FD4B}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9EF9846-2814-438B-8079-0C684926AF58}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78FB3D33-78AD-40B8-B93D-6C48166AC844}"/>
 </file>
</xml_diff>